<commit_message>
worked on portfolio, performance measurements improved
</commit_message>
<xml_diff>
--- a/Portfolio/effizienz_tabelle.xlsx
+++ b/Portfolio/effizienz_tabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwein\Documents\GitHub\EFI\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC157443-7350-4ECB-A964-9AFC4970C526}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD47307-E99E-431D-882E-6FD9472BC57B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{362BBB06-4FA3-40E8-AF72-36A04FA32FD8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>depth</t>
   </si>
@@ -54,16 +54,10 @@
     <t>Drachenkurve</t>
   </si>
   <si>
-    <t>log4(moveCount)</t>
-  </si>
-  <si>
     <t>log3(moveCount)</t>
   </si>
   <si>
     <t>duration/moveCount</t>
-  </si>
-  <si>
-    <t>log4(duration)</t>
   </si>
   <si>
     <t>log2(moveCount)</t>
@@ -75,7 +69,37 @@
     <t>log2(duration)</t>
   </si>
   <si>
-    <t>duration (ms)</t>
+    <t>Stufe</t>
+  </si>
+  <si>
+    <t>Laufzeit (ms)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>s = Move count</t>
+  </si>
+  <si>
+    <t>log4(s)</t>
+  </si>
+  <si>
+    <t>Laufzeit/s</t>
+  </si>
+  <si>
+    <t>&gt; line?</t>
+  </si>
+  <si>
+    <t>log4(Laufzeit)</t>
+  </si>
+  <si>
+    <t>Plot:</t>
+  </si>
+  <si>
+    <t>Stufe:log(Laufzeit)</t>
+  </si>
+  <si>
+    <t>Laufzeit ungeteilt</t>
   </si>
 </sst>
 </file>
@@ -102,12 +126,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,12 +152,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -230,7 +262,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>depth</c:v>
+                  <c:v>Stufe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -292,11 +324,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$6</c:f>
+              <c:f>Tabelle1!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>duration (ms)</c:v>
+                  <c:v>Laufzeit (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -318,31 +350,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>239</c:v>
+                  <c:v>565</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0">
-                  <c:v>813.66666666666663</c:v>
+                  <c:v>2378</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0">
-                  <c:v>4824.333333333333</c:v>
+                  <c:v>9512</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0">
-                  <c:v>29673.333333333332</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0">
-                  <c:v>97133</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0">
-                  <c:v>398885</c:v>
+                  <c:v>40531</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>174195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>629783</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,11 +390,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$E$6</c:f>
+              <c:f>Tabelle1!$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>moveCount</c:v>
+                  <c:v>s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -379,7 +411,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$7:$E$15</c:f>
+              <c:f>Tabelle1!$F$7:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1174,7 +1206,7 @@
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
@@ -1502,7 +1534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A3CE31-6E04-4DE6-B48E-EE2396E24816}">
-  <dimension ref="C4:V15"/>
+  <dimension ref="A2:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="86" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
@@ -1510,655 +1542,703 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="N6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="P6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="V6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4">
+        <f>D7/3</f>
+        <v>8</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <f>LOG(D7,4)</f>
-        <v>2.1609640474436813</v>
-      </c>
-      <c r="G7">
-        <f>LOG(E7,4)</f>
+        <v>2.2924812503605785</v>
+      </c>
+      <c r="H7">
+        <f>LOG(F7,4)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="2">
-        <f>D7/E7</f>
-        <v>20</v>
-      </c>
-      <c r="J7">
+      <c r="I7" s="6">
+        <f>D7/F7</f>
+        <v>24</v>
+      </c>
+      <c r="K7">
         <v>0</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>29</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="M7">
+      <c r="N7">
+        <f>LOG(M7,3)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
         <f>LOG(L7,3)</f>
+        <v>3.0650447521106625</v>
+      </c>
+      <c r="P7" s="2">
+        <f>L7/M7</f>
+        <v>29</v>
+      </c>
+      <c r="R7">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
-        <f>LOG(K7,3)</f>
-        <v>3.0650447521106625</v>
-      </c>
-      <c r="O7" s="2">
-        <f>K7/L7</f>
-        <v>29</v>
-      </c>
-      <c r="Q7">
+      <c r="S7">
+        <v>12</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <f>LOG(T7,2)</f>
         <v>0</v>
       </c>
-      <c r="R7">
+      <c r="V7" s="3">
+        <f>LOG(S7,2)</f>
+        <v>3.5849625007211565</v>
+      </c>
+      <c r="W7" s="2">
+        <f>S7/T7</f>
         <v>12</v>
       </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <f>LOG(S7,2)</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="3">
-        <f>LOG(R7,2)</f>
-        <v>3.5849625007211565</v>
-      </c>
-      <c r="V7" s="2">
-        <f>R7/S7</f>
-        <v>12</v>
-      </c>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <f>87/3</f>
-        <v>29</v>
-      </c>
-      <c r="E8">
+        <v>39</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" ref="E8:E15" si="0">D8/3</f>
+        <v>13</v>
+      </c>
+      <c r="F8">
         <v>4</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <f>LOG(D8,4)</f>
-        <v>2.4289904975637864</v>
-      </c>
-      <c r="G8">
-        <f>LOG(E8,4)</f>
+        <v>2.6427011094311244</v>
+      </c>
+      <c r="H8">
+        <f>LOG(F8,4)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="2">
-        <f t="shared" ref="H8:H15" si="0">D8/E8</f>
-        <v>7.25</v>
-      </c>
-      <c r="J8">
+      <c r="I8" s="6">
+        <f>D8/F8</f>
+        <v>9.75</v>
+      </c>
+      <c r="K8">
         <v>1</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>33</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>3</v>
       </c>
-      <c r="M8">
-        <f t="shared" ref="M8:M15" si="1">LOG(L8,3)</f>
+      <c r="N8">
+        <f t="shared" ref="N8:N15" si="1">LOG(M8,3)</f>
         <v>1</v>
       </c>
-      <c r="N8" s="3">
-        <f t="shared" ref="N8:N15" si="2">LOG(K8,3)</f>
+      <c r="O8" s="3">
+        <f t="shared" ref="O8:O15" si="2">LOG(L8,3)</f>
         <v>3.1826583386441376</v>
       </c>
-      <c r="O8" s="2">
-        <f t="shared" ref="O7:O15" si="3">K8/L8</f>
+      <c r="P8" s="2">
+        <f t="shared" ref="P7:P15" si="3">L8/M8</f>
         <v>11</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>2</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>24</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>4</v>
       </c>
-      <c r="T8">
-        <f t="shared" ref="T8:T14" si="4">LOG(S8,2)</f>
+      <c r="U8">
+        <f t="shared" ref="U8:U14" si="4">LOG(T8,2)</f>
         <v>2</v>
       </c>
-      <c r="U8" s="3">
-        <f t="shared" ref="U8:U14" si="5">LOG(R8,2)</f>
+      <c r="V8" s="3">
+        <f t="shared" ref="V8:V14" si="5">LOG(S8,2)</f>
         <v>4.584962500721157</v>
       </c>
-      <c r="V8" s="2">
-        <f t="shared" ref="V8:V14" si="6">R8/S8</f>
+      <c r="W8" s="2">
+        <f t="shared" ref="W8:W14" si="6">S8/T8</f>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
-        <f>225/3</f>
-        <v>75</v>
-      </c>
-      <c r="E9">
+        <v>148</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>49.333333333333336</v>
+      </c>
+      <c r="F9">
         <v>16</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <f>LOG(D9,4)</f>
-        <v>3.1144093452479402</v>
-      </c>
-      <c r="G9">
-        <f>LOG(E9,4)</f>
+        <v>3.6047266828144746</v>
+      </c>
+      <c r="H9">
+        <f>LOG(F9,4)</f>
         <v>2</v>
       </c>
-      <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6875</v>
-      </c>
-      <c r="J9">
+      <c r="I9" s="6">
+        <f>D9/F9</f>
+        <v>9.25</v>
+      </c>
+      <c r="K9">
         <v>2</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>59</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>9</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="3">
         <f t="shared" si="2"/>
         <v>3.7115345294827136</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <f t="shared" si="3"/>
         <v>6.5555555555555554</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>4</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>80</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>16</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="U9" s="3">
+      <c r="V9" s="3">
         <f t="shared" si="5"/>
         <v>6.3219280948873617</v>
       </c>
-      <c r="V9" s="2">
+      <c r="W9" s="2">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10">
-        <f>717/3</f>
-        <v>239</v>
-      </c>
-      <c r="E10">
+        <v>565</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>188.33333333333334</v>
+      </c>
+      <c r="F10">
         <v>64</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <f>LOG(D10,4)</f>
-        <v>3.9504334039903748</v>
-      </c>
-      <c r="G10">
-        <f>LOG(E10,4)</f>
+        <v>4.5710535286512757</v>
+      </c>
+      <c r="H10">
+        <f>LOG(F10,4)</f>
         <v>3</v>
       </c>
-      <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>3.734375</v>
-      </c>
-      <c r="J10">
+      <c r="I10" s="6">
+        <f>D10/F10</f>
+        <v>8.828125</v>
+      </c>
+      <c r="K10">
         <v>3</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>126</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>27</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N10" s="3">
+      <c r="O10" s="3">
         <f t="shared" si="2"/>
         <v>4.4021735027328797</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <f t="shared" si="3"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>6</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>225</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>64</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="U10" s="3">
+      <c r="V10" s="3">
         <f t="shared" si="5"/>
         <v>7.8137811912170374</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <f t="shared" si="6"/>
         <v>3.515625</v>
       </c>
     </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11" s="4">
-        <f>2441/3</f>
-        <v>813.66666666666663</v>
-      </c>
-      <c r="E11">
+        <v>2378</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>792.66666666666663</v>
+      </c>
+      <c r="F11">
         <f>768/3</f>
         <v>256</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <f>LOG(D11,4)</f>
-        <v>4.8341470395299986</v>
-      </c>
-      <c r="G11">
-        <f>LOG(E11,4)</f>
+        <v>5.6077664998728283</v>
+      </c>
+      <c r="H11">
+        <f>LOG(F11,4)</f>
         <v>4</v>
       </c>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>3.1783854166666665</v>
-      </c>
-      <c r="J11">
+      <c r="I11" s="6">
+        <f>D11/F11</f>
+        <v>9.2890625</v>
+      </c>
+      <c r="K11">
         <v>4</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>317</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>81</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="N11" s="3">
+      <c r="O11" s="3">
         <f t="shared" si="2"/>
         <v>5.2419782968739774</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <f t="shared" si="3"/>
         <v>3.9135802469135803</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>8</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>659</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>256</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="U11" s="3">
+      <c r="V11" s="3">
         <f t="shared" si="5"/>
         <v>9.3641346550080513</v>
       </c>
-      <c r="V11" s="2">
+      <c r="W11" s="2">
         <f t="shared" si="6"/>
         <v>2.57421875</v>
       </c>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C12">
         <v>5</v>
       </c>
       <c r="D12" s="4">
-        <f>14473/3</f>
-        <v>4824.333333333333</v>
-      </c>
-      <c r="E12">
-        <f>E11*4</f>
+        <v>9512</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>3170.6666666666665</v>
+      </c>
+      <c r="F12">
+        <f>F11*4</f>
         <v>1024</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <f>LOG(D12,4)</f>
-        <v>6.1180569385840542</v>
-      </c>
-      <c r="G12">
-        <f>LOG(E12,4)</f>
+        <v>6.6077664998728283</v>
+      </c>
+      <c r="H12">
+        <f>LOG(F12,4)</f>
         <v>5</v>
       </c>
-      <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>4.711263020833333</v>
-      </c>
-      <c r="J12">
+      <c r="I12" s="6">
+        <f>D12/F12</f>
+        <v>9.2890625</v>
+      </c>
+      <c r="K12">
         <v>5</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>945</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>243</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f t="shared" si="1"/>
         <v>4.9999999999999991</v>
       </c>
-      <c r="N12" s="3">
+      <c r="O12" s="3">
         <f t="shared" si="2"/>
         <v>6.236217269879349</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2">
         <f t="shared" si="3"/>
         <v>3.8888888888888888</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>10</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>2600</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>1024</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="U12" s="3">
+      <c r="V12" s="3">
         <f t="shared" si="5"/>
         <v>11.344295907915818</v>
       </c>
-      <c r="V12" s="2">
+      <c r="W12" s="2">
         <f t="shared" si="6"/>
         <v>2.5390625</v>
       </c>
     </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C13">
         <v>6</v>
       </c>
       <c r="D13" s="4">
-        <f>89020/3</f>
-        <v>29673.333333333332</v>
-      </c>
-      <c r="E13">
-        <f t="shared" ref="E13:E15" si="7">E12*4</f>
+        <v>40531</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>13510.333333333334</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F15" si="7">F12*4</f>
         <v>4096</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <f>LOG(D13,4)</f>
-        <v>7.4284396898092373</v>
-      </c>
-      <c r="G13">
-        <f>LOG(E13,4)</f>
+        <v>7.6533690751138241</v>
+      </c>
+      <c r="H13">
+        <f>LOG(F13,4)</f>
         <v>6</v>
       </c>
-      <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>7.244466145833333</v>
-      </c>
-      <c r="J13">
+      <c r="I13" s="6">
+        <f>D13/F13</f>
+        <v>9.895263671875</v>
+      </c>
+      <c r="K13">
         <v>6</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>2278</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>729</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="N13" s="3">
+      <c r="O13" s="3">
         <f t="shared" si="2"/>
         <v>7.0371078348120264</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <f t="shared" si="3"/>
         <v>3.1248285322359397</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>12</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>10346</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>4096</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="U13" s="3">
+      <c r="V13" s="3">
         <f t="shared" si="5"/>
         <v>13.336785476203755</v>
       </c>
-      <c r="V13" s="2">
+      <c r="W13" s="2">
         <f t="shared" si="6"/>
         <v>2.52587890625</v>
       </c>
     </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C14">
         <v>7</v>
       </c>
-      <c r="D14" s="4">
-        <f>291399/3</f>
-        <v>97133</v>
-      </c>
-      <c r="E14">
+      <c r="D14">
+        <v>174195</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>58065</v>
+      </c>
+      <c r="F14">
         <f>49152/3</f>
         <v>16384</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <f>LOG(D14,4)</f>
-        <v>8.2838369501000226</v>
-      </c>
-      <c r="G14">
-        <f>LOG(E14,4)</f>
+        <v>8.7051718443109927</v>
+      </c>
+      <c r="H14">
+        <f>LOG(F14,4)</f>
         <v>7</v>
       </c>
-      <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>5.92852783203125</v>
-      </c>
-      <c r="J14">
+      <c r="I14" s="6">
+        <f>D14/F14</f>
+        <v>10.63201904296875</v>
+      </c>
+      <c r="K14">
         <v>7</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>10574</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>2187</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="N14" s="3">
+      <c r="O14" s="3">
         <f t="shared" si="2"/>
         <v>8.4344163381142518</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <f t="shared" si="3"/>
         <v>4.8349336991312297</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>14</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>86928</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>16384</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="U14" s="3">
+      <c r="V14" s="3">
         <f t="shared" si="5"/>
         <v>16.407533331671324</v>
       </c>
-      <c r="V14" s="2">
+      <c r="W14" s="2">
         <f t="shared" si="6"/>
         <v>5.3056640625</v>
       </c>
     </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C15">
         <v>8</v>
       </c>
-      <c r="D15" s="4">
-        <v>398885</v>
-      </c>
-      <c r="E15">
+      <c r="D15">
+        <v>629783</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>209927.66666666666</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="7"/>
         <v>65536</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <f>LOG(D15,4)</f>
-        <v>9.3028066732948194</v>
-      </c>
-      <c r="G15">
-        <f>LOG(E15,4)</f>
+        <v>9.6322476445778769</v>
+      </c>
+      <c r="H15">
+        <f>LOG(F15,4)</f>
         <v>8</v>
       </c>
-      <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>6.0865020751953125</v>
-      </c>
-      <c r="J15">
+      <c r="I15" s="6">
+        <f>D15/F15</f>
+        <v>9.6097259521484375</v>
+      </c>
+      <c r="K15">
         <v>8</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>48256</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>6561</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="N15" s="3">
+      <c r="O15" s="3">
         <f t="shared" si="2"/>
         <v>9.8162705465836577</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <f t="shared" si="3"/>
         <v>7.3549763755525071</v>
       </c>
-      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>